<commit_message>
updated code for matching algorithm
</commit_message>
<xml_diff>
--- a/(12) City_JUNusage_Aug-bill.xlsx
+++ b/(12) City_JUNusage_Aug-bill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/labuser/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/labuser/Desktop/OESUtilityChecker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0A65EE-D50F-0445-87D4-EFAA0311A700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A612D1-76CF-C142-8EA6-99B1A80AB4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1780" windowWidth="14000" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11440" yWindow="580" windowWidth="15600" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBERLIN" sheetId="1" r:id="rId1"/>
@@ -1642,7 +1642,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1846,6 +1846,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -2024,7 +2030,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2054,6 +2060,7 @@
     <xf numFmtId="44" fontId="16" fillId="36" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="37" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2414,8 +2421,8 @@
   <dimension ref="A1:N252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B169" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9226,10 +9233,10 @@
       <c r="E155" s="2">
         <v>1000</v>
       </c>
-      <c r="F155" s="11">
+      <c r="F155" s="21">
         <v>97.9</v>
       </c>
-      <c r="G155" s="11">
+      <c r="G155" s="21">
         <v>71.099999999999994</v>
       </c>
       <c r="H155" s="11">
@@ -12650,35 +12657,35 @@
       <c r="C233" s="7"/>
       <c r="D233" s="7"/>
       <c r="E233" s="7">
-        <f>SUM(E2:E232)</f>
+        <f t="shared" ref="E233:L233" si="0">SUM(E2:E232)</f>
         <v>340500</v>
       </c>
       <c r="F233" s="9">
-        <f>SUM(F2:F232)</f>
+        <f t="shared" si="0"/>
         <v>34700.679999999964</v>
       </c>
       <c r="G233" s="9">
-        <f>SUM(G2:G232)</f>
+        <f t="shared" si="0"/>
         <v>22407.150000000031</v>
       </c>
       <c r="H233" s="9">
-        <f>SUM(H2:H232)</f>
+        <f t="shared" si="0"/>
         <v>10076.39</v>
       </c>
       <c r="I233" s="7">
-        <f>SUM(I2:I232)</f>
+        <f t="shared" si="0"/>
         <v>2193950</v>
       </c>
       <c r="J233" s="9">
-        <f>SUM(J2:J232)</f>
+        <f t="shared" si="0"/>
         <v>280484.12999999995</v>
       </c>
       <c r="K233" s="7">
-        <f>SUM(K2:K232)</f>
+        <f t="shared" si="0"/>
         <v>5602.0999999999995</v>
       </c>
       <c r="L233" s="9">
-        <f>SUM(L2:L232)</f>
+        <f t="shared" si="0"/>
         <v>347668.35000000003</v>
       </c>
       <c r="M233" s="7"/>
@@ -13392,27 +13399,27 @@
       <c r="C250" s="7"/>
       <c r="D250" s="7"/>
       <c r="E250" s="7">
-        <f t="shared" ref="E250:J250" si="0">SUM(E235:E249)</f>
+        <f t="shared" ref="E250:J250" si="1">SUM(E235:E249)</f>
         <v>2000</v>
       </c>
       <c r="F250" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>342.65</v>
       </c>
       <c r="G250" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>248.85000000000002</v>
       </c>
       <c r="H250" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>106.25</v>
       </c>
       <c r="I250" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5564</v>
       </c>
       <c r="J250" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>841.95999999999992</v>
       </c>
       <c r="K250" s="7"/>
@@ -13424,27 +13431,27 @@
     </row>
     <row r="252" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E252">
-        <f t="shared" ref="E252:J252" si="1">E250+E233</f>
+        <f t="shared" ref="E252:J252" si="2">E250+E233</f>
         <v>342500</v>
       </c>
       <c r="F252" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35043.329999999965</v>
       </c>
       <c r="G252" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22656.000000000029</v>
       </c>
       <c r="H252" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10182.64</v>
       </c>
       <c r="I252" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2199514</v>
       </c>
       <c r="J252" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>281326.08999999997</v>
       </c>
       <c r="K252" s="11"/>

</xml_diff>